<commit_message>
terminado diccionariod e datos, mer y psaje a tablas, faltan los inserts y la creacion
</commit_message>
<xml_diff>
--- a/ProyectoMaterias/Base de Datos/CorreccionesBD/BlindsTech-diccionarioDatos.xlsx
+++ b/ProyectoMaterias/Base de Datos/CorreccionesBD/BlindsTech-diccionarioDatos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Atributo</t>
   </si>
@@ -160,13 +160,6 @@
     <t>PK, NOT NULL, IDENTITY {1,1}</t>
   </si>
   <si>
-    <t>cant_casas</t>
-  </si>
-  <si>
-    <t>Cantidad de casas que se pueden
-vincular al servicio</t>
-  </si>
-  <si>
     <t>Nombre del servicio</t>
   </si>
   <si>
@@ -174,9 +167,6 @@
   </si>
   <si>
     <t>TEXT</t>
-  </si>
-  <si>
-    <t>descripcion gdel servicio</t>
   </si>
   <si>
     <t>Contrato</t>
@@ -216,9 +206,6 @@
     <t>BIT</t>
   </si>
   <si>
-    <t>si el contrato exipró o no</t>
-  </si>
-  <si>
     <t>id_rpis</t>
   </si>
   <si>
@@ -234,18 +221,12 @@
     <t>RPIs</t>
   </si>
   <si>
-    <t>nombre_serie</t>
-  </si>
-  <si>
     <t>Nombre de serie de la RaspBerry PI</t>
   </si>
   <si>
     <t>estado</t>
   </si>
   <si>
-    <t>NOT NULL, CHECK(estado IN(habilitada, deshabilitada, en funcionamiento, apagada))</t>
-  </si>
-  <si>
     <t>estados de la RPI</t>
   </si>
   <si>
@@ -258,9 +239,6 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>NOT NULL, CHECK(tipo IN(americana, toldo, corrediza, polea))</t>
-  </si>
-  <si>
     <t>tipo de persianas</t>
   </si>
   <si>
@@ -289,6 +267,33 @@
   </si>
   <si>
     <t>Tipo de empleado</t>
+  </si>
+  <si>
+    <t>NOT NULL, CHECK(tipo IN ('tecnicos', 'administrativos'))</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>Precio del servicio</t>
+  </si>
+  <si>
+    <t>descripcion del servicio</t>
+  </si>
+  <si>
+    <t>Si el contrato exipró o no</t>
+  </si>
+  <si>
+    <t>numero_serie</t>
+  </si>
+  <si>
+    <t>NOT NULL, CHECK(estado IN('habilitada', 'deshabilitada', 'en funcionamiento', 'apagada'))</t>
+  </si>
+  <si>
+    <t>NOT NULL, CHECK(tipo IN('americana', 'toldo', 'corrediza', 'polea'))</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
@@ -433,13 +438,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,12 +800,12 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -885,12 +890,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -934,27 +939,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>77</v>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>11</v>
+      <c r="C17" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -985,12 +990,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1027,20 +1032,18 @@
       <c r="B28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -1056,59 +1059,57 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
     </row>
     <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>6</v>
@@ -1117,12 +1118,12 @@
         <v>26</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>6</v>
@@ -1131,12 +1132,12 @@
         <v>26</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>17</v>
@@ -1145,40 +1146,40 @@
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>6</v>
@@ -1187,16 +1188,16 @@
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
+      <c r="A47" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
@@ -1209,12 +1210,12 @@
         <v>26</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>6</v>
@@ -1223,16 +1224,16 @@
         <v>26</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
+      <c r="A52" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
@@ -1250,7 +1251,7 @@
     </row>
     <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>14</v>
@@ -1259,34 +1260,34 @@
         <v>11</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
+      <c r="A58" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
     </row>
     <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>6</v>
@@ -1300,29 +1301,29 @@
     </row>
     <row r="60" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="A63" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
     </row>
     <row r="64" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>6</v>
@@ -1331,26 +1332,24 @@
         <v>26</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>17</v>
@@ -1359,12 +1358,12 @@
         <v>11</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>6</v>
@@ -1373,26 +1372,26 @@
         <v>31</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
+      <c r="A70" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
     </row>
     <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>38</v>
@@ -1400,7 +1399,7 @@
     </row>
     <row r="72" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>6</v>
@@ -1409,12 +1408,12 @@
         <v>26</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>10</v>
@@ -1423,22 +1422,22 @@
         <v>11</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A63:D63"/>
     <mergeCell ref="A70:D70"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A31:D31"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A63:D63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TERMINADAS LAS CORRECCIONES DE BD, ESTA PARA REVISAR
</commit_message>
<xml_diff>
--- a/ProyectoMaterias/Base de Datos/CorreccionesBD/BlindsTech-diccionarioDatos.xlsx
+++ b/ProyectoMaterias/Base de Datos/CorreccionesBD/BlindsTech-diccionarioDatos.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -770,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>